<commit_message>
updated compare models function
</commit_message>
<xml_diff>
--- a/Results/word2vec_top_category_combinations.xlsx
+++ b/Results/word2vec_top_category_combinations.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3931</v>
+        <v>3916</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3701</v>
+        <v>3677</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2779</v>
+        <v>2816</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1970</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="6">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>814</v>
+        <v>816</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>601</v>
+        <v>579</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>554</v>
+        <v>550</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>520</v>
+        <v>498</v>
       </c>
     </row>
     <row r="11">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>484</v>
+        <v>497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>